<commit_message>
Qiu ethan patch 1 (#8)
更新module
統一名稱命名

Co-authored-by: Tony Yao <tony24862486@gmail.com>
</commit_message>
<xml_diff>
--- a/foxlink_dispatch/test_data/D5X device事件簿.xlsx
+++ b/foxlink_dispatch/test_data/D5X device事件簿.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20383"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anderson/Desktop/台科大資料/20210716台科資料提供/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ethan\SimsLab\正崴 Foxlink\#台科團隊\foxlink_dispatch\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E901F5-652E-4506-8C4E-EB649C183187}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2140" windowWidth="28800" windowHeight="12440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2145" windowWidth="28800" windowHeight="12435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device_1" sheetId="3" r:id="rId1"/>
@@ -58,71 +59,71 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="AOI" type="6" refreshedVersion="2" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="AOI" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/AOI.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="Barcode" type="6" refreshedVersion="2" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="Barcode" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/Barcode.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="ChipAssy" type="6" refreshedVersion="2" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="ChipAssy" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/ChipAssy.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="Glue" type="6" refreshedVersion="2" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="Glue" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/Glue.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="LeakTest" type="6" refreshedVersion="2" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="LeakTest" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/LeakTest.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="OS" type="6" refreshedVersion="2" background="1" saveData="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="OS" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/OS.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="Package" type="6" refreshedVersion="2" background="1" saveData="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="Package" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/Package.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="Plug" type="6" refreshedVersion="2" background="1" saveData="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="Plug" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/Plug.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="ShellAssy" type="6" refreshedVersion="2" background="1" saveData="1">
+  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="ShellAssy" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/ShellAssy.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="Tray" type="6" refreshedVersion="2" background="1" saveData="1">
+  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" name="Tray" type="6" refreshedVersion="2" background="1" saveData="1">
     <textPr sourceFile="/Users/anderson/Downloads/Tray.csv" comma="1">
       <textFields>
         <textField/>
@@ -1008,7 +1009,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1226,48 +1227,51 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Plug" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Plug" connectionId="8" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Package" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Package" connectionId="7" xr16:uid="{00000000-0016-0000-0900-000009000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tray" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Tray" connectionId="10" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Glue" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Glue" connectionId="4" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ChipAssy" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ChipAssy" connectionId="3" xr16:uid="{00000000-0016-0000-0300-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShellAssy" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ShellAssy" connectionId="9" xr16:uid="{00000000-0016-0000-0400-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Barcode" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Barcode" connectionId="2" xr16:uid="{00000000-0016-0000-0500-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OS" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OS" connectionId="6" xr16:uid="{00000000-0016-0000-0600-000006000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LeakTest" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="LeakTest" connectionId="5" xr16:uid="{00000000-0016-0000-0700-000007000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="AOI" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="AOI" connectionId="1" xr16:uid="{00000000-0016-0000-0800-000008000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1527,22 +1531,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="26.125" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>288</v>
       </c>
@@ -1556,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>171</v>
       </c>
@@ -1568,7 +1572,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>172</v>
       </c>
@@ -1580,7 +1584,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>173</v>
       </c>
@@ -1592,7 +1596,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>174</v>
       </c>
@@ -1604,7 +1608,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>175</v>
       </c>
@@ -1616,7 +1620,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>176</v>
       </c>
@@ -1628,7 +1632,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>177</v>
       </c>
@@ -1640,7 +1644,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>178</v>
       </c>
@@ -1652,7 +1656,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>179</v>
       </c>
@@ -1664,7 +1668,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>180</v>
       </c>
@@ -1676,7 +1680,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>181</v>
       </c>
@@ -1688,7 +1692,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>182</v>
       </c>
@@ -1700,7 +1704,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>183</v>
       </c>
@@ -1712,7 +1716,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>184</v>
       </c>
@@ -1724,7 +1728,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>185</v>
       </c>
@@ -1736,7 +1740,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>186</v>
       </c>
@@ -1748,7 +1752,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>187</v>
       </c>
@@ -1760,7 +1764,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>188</v>
       </c>
@@ -1772,7 +1776,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>189</v>
       </c>
@@ -1784,7 +1788,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>190</v>
       </c>
@@ -1796,7 +1800,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>191</v>
       </c>
@@ -1808,7 +1812,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>192</v>
       </c>
@@ -1820,7 +1824,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>193</v>
       </c>
@@ -1832,7 +1836,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>194</v>
       </c>
@@ -1844,7 +1848,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>195</v>
       </c>
@@ -1856,7 +1860,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>200</v>
       </c>
@@ -1866,7 +1870,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>201</v>
       </c>
@@ -1876,7 +1880,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>202</v>
       </c>
@@ -1886,7 +1890,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>203</v>
       </c>
@@ -1896,7 +1900,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>205</v>
       </c>
@@ -1906,7 +1910,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>210</v>
       </c>
@@ -1918,7 +1922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>211</v>
       </c>
@@ -1928,7 +1932,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>215</v>
       </c>
@@ -1938,7 +1942,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>216</v>
       </c>
@@ -1948,7 +1952,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>217</v>
       </c>
@@ -1958,7 +1962,7 @@
       <c r="C36" s="1"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>218</v>
       </c>
@@ -1968,7 +1972,7 @@
       <c r="C37" s="1"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>219</v>
       </c>
@@ -1978,7 +1982,7 @@
       <c r="C38" s="1"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>250</v>
       </c>
@@ -1991,26 +1995,27 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="24.875" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>288</v>
       </c>
@@ -2024,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>44</v>
       </c>
@@ -2036,7 +2041,7 @@
       </c>
       <c r="D2" s="17"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>45</v>
       </c>
@@ -2048,7 +2053,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>46</v>
       </c>
@@ -2060,7 +2065,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>47</v>
       </c>
@@ -2072,7 +2077,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>48</v>
       </c>
@@ -2084,7 +2089,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>49</v>
       </c>
@@ -2096,7 +2101,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>50</v>
       </c>
@@ -2108,7 +2113,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>51</v>
       </c>
@@ -2120,7 +2125,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>190</v>
       </c>
@@ -2132,7 +2137,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>191</v>
       </c>
@@ -2144,7 +2149,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>192</v>
       </c>
@@ -2156,7 +2161,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>198</v>
       </c>
@@ -2168,7 +2173,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>200</v>
       </c>
@@ -2178,7 +2183,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>201</v>
       </c>
@@ -2188,7 +2193,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>202</v>
       </c>
@@ -2198,7 +2203,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>203</v>
       </c>
@@ -2208,7 +2213,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>205</v>
       </c>
@@ -2218,7 +2223,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>210</v>
       </c>
@@ -2228,7 +2233,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>211</v>
       </c>
@@ -2238,7 +2243,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>215</v>
       </c>
@@ -2248,7 +2253,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>216</v>
       </c>
@@ -2258,7 +2263,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>217</v>
       </c>
@@ -2268,7 +2273,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>218</v>
       </c>
@@ -2278,7 +2283,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>219</v>
       </c>
@@ -2288,7 +2293,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>250</v>
       </c>
@@ -2305,22 +2310,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="24.125" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>288</v>
       </c>
@@ -2334,7 +2339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>171</v>
       </c>
@@ -2346,7 +2351,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>172</v>
       </c>
@@ -2358,7 +2363,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>173</v>
       </c>
@@ -2370,7 +2375,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>174</v>
       </c>
@@ -2382,7 +2387,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>175</v>
       </c>
@@ -2394,7 +2399,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>176</v>
       </c>
@@ -2406,7 +2411,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>177</v>
       </c>
@@ -2418,7 +2423,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>178</v>
       </c>
@@ -2430,7 +2435,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>179</v>
       </c>
@@ -2442,7 +2447,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>180</v>
       </c>
@@ -2454,7 +2459,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>181</v>
       </c>
@@ -2466,7 +2471,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>182</v>
       </c>
@@ -2478,7 +2483,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>183</v>
       </c>
@@ -2490,7 +2495,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>190</v>
       </c>
@@ -2502,7 +2507,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>191</v>
       </c>
@@ -2514,7 +2519,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>192</v>
       </c>
@@ -2526,7 +2531,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>200</v>
       </c>
@@ -2536,7 +2541,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>201</v>
       </c>
@@ -2546,7 +2551,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>202</v>
       </c>
@@ -2556,7 +2561,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>203</v>
       </c>
@@ -2566,7 +2571,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>205</v>
       </c>
@@ -2576,7 +2581,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>210</v>
       </c>
@@ -2586,7 +2591,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>211</v>
       </c>
@@ -2596,7 +2601,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>215</v>
       </c>
@@ -2606,7 +2611,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>216</v>
       </c>
@@ -2616,7 +2621,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>217</v>
       </c>
@@ -2626,7 +2631,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>218</v>
       </c>
@@ -2636,7 +2641,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>219</v>
       </c>
@@ -2646,7 +2651,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>250</v>
       </c>
@@ -2663,22 +2668,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>288</v>
       </c>
@@ -2692,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2704,7 +2709,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2716,7 +2721,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2728,7 +2733,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2740,7 +2745,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -2752,7 +2757,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2764,7 +2769,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2776,7 +2781,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2788,7 +2793,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -2800,7 +2805,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2812,7 +2817,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2824,7 +2829,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2836,7 +2841,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2848,7 +2853,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2860,7 +2865,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>21</v>
       </c>
@@ -2872,7 +2877,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>30</v>
       </c>
@@ -2884,7 +2889,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>31</v>
       </c>
@@ -2896,7 +2901,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>32</v>
       </c>
@@ -2908,7 +2913,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>190</v>
       </c>
@@ -2920,7 +2925,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>191</v>
       </c>
@@ -2932,7 +2937,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>198</v>
       </c>
@@ -2944,7 +2949,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>200</v>
       </c>
@@ -2954,7 +2959,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>201</v>
       </c>
@@ -2964,7 +2969,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>202</v>
       </c>
@@ -2974,7 +2979,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>203</v>
       </c>
@@ -2984,7 +2989,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>205</v>
       </c>
@@ -2994,7 +2999,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>210</v>
       </c>
@@ -3004,7 +3009,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>211</v>
       </c>
@@ -3014,7 +3019,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>215</v>
       </c>
@@ -3024,7 +3029,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>216</v>
       </c>
@@ -3034,7 +3039,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>217</v>
       </c>
@@ -3044,7 +3049,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>218</v>
       </c>
@@ -3054,7 +3059,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>219</v>
       </c>
@@ -3064,7 +3069,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>250</v>
       </c>
@@ -3081,22 +3086,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>288</v>
       </c>
@@ -3110,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3122,7 +3127,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3134,7 +3139,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3146,7 +3151,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3158,7 +3163,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3170,7 +3175,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3182,7 +3187,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3194,7 +3199,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3206,7 +3211,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3218,7 +3223,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3230,7 +3235,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3242,7 +3247,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3254,7 +3259,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -3266,7 +3271,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -3278,7 +3283,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -3290,7 +3295,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -3302,7 +3307,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -3314,7 +3319,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>34</v>
       </c>
@@ -3326,7 +3331,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>35</v>
       </c>
@@ -3338,7 +3343,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>36</v>
       </c>
@@ -3350,7 +3355,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>37</v>
       </c>
@@ -3362,7 +3367,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>38</v>
       </c>
@@ -3374,7 +3379,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>190</v>
       </c>
@@ -3386,7 +3391,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>191</v>
       </c>
@@ -3398,7 +3403,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>192</v>
       </c>
@@ -3410,7 +3415,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>193</v>
       </c>
@@ -3422,7 +3427,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>198</v>
       </c>
@@ -3436,7 +3441,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>200</v>
       </c>
@@ -3446,7 +3451,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>201</v>
       </c>
@@ -3456,7 +3461,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>202</v>
       </c>
@@ -3466,7 +3471,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>203</v>
       </c>
@@ -3476,7 +3481,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>205</v>
       </c>
@@ -3486,7 +3491,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>210</v>
       </c>
@@ -3496,7 +3501,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>211</v>
       </c>
@@ -3506,7 +3511,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>215</v>
       </c>
@@ -3516,7 +3521,7 @@
       <c r="C36" s="1"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>216</v>
       </c>
@@ -3526,7 +3531,7 @@
       <c r="C37" s="1"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>217</v>
       </c>
@@ -3536,7 +3541,7 @@
       <c r="C38" s="1"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>218</v>
       </c>
@@ -3546,7 +3551,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>219</v>
       </c>
@@ -3556,7 +3561,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>250</v>
       </c>
@@ -3573,22 +3578,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView zoomScale="108" zoomScaleNormal="108" zoomScalePageLayoutView="108" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="30.375" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>288</v>
       </c>
@@ -3602,7 +3607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3614,7 +3619,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3626,7 +3631,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3638,7 +3643,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3650,7 +3655,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3662,7 +3667,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3674,7 +3679,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3686,7 +3691,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3698,7 +3703,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3710,7 +3715,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3722,7 +3727,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3734,7 +3739,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3746,7 +3751,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -3758,7 +3763,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -3770,7 +3775,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>18</v>
       </c>
@@ -3782,7 +3787,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>19</v>
       </c>
@@ -3794,7 +3799,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>20</v>
       </c>
@@ -3806,7 +3811,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>21</v>
       </c>
@@ -3818,7 +3823,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>22</v>
       </c>
@@ -3830,7 +3835,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>23</v>
       </c>
@@ -3842,7 +3847,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>24</v>
       </c>
@@ -3854,7 +3859,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>25</v>
       </c>
@@ -3866,7 +3871,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>26</v>
       </c>
@@ -3878,7 +3883,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>27</v>
       </c>
@@ -3890,7 +3895,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>28</v>
       </c>
@@ -3902,7 +3907,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>54</v>
       </c>
@@ -3914,7 +3919,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>190</v>
       </c>
@@ -3926,7 +3931,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>191</v>
       </c>
@@ -3938,7 +3943,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>192</v>
       </c>
@@ -3950,7 +3955,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>193</v>
       </c>
@@ -3962,7 +3967,7 @@
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>194</v>
       </c>
@@ -3974,7 +3979,7 @@
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>198</v>
       </c>
@@ -3988,7 +3993,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>200</v>
       </c>
@@ -3998,7 +4003,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>201</v>
       </c>
@@ -4008,7 +4013,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>202</v>
       </c>
@@ -4018,7 +4023,7 @@
       <c r="C36" s="1"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>203</v>
       </c>
@@ -4028,7 +4033,7 @@
       <c r="C37" s="1"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>205</v>
       </c>
@@ -4038,7 +4043,7 @@
       <c r="C38" s="1"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>210</v>
       </c>
@@ -4048,7 +4053,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>211</v>
       </c>
@@ -4058,7 +4063,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>215</v>
       </c>
@@ -4068,7 +4073,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>216</v>
       </c>
@@ -4078,7 +4083,7 @@
       <c r="C42" s="1"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>217</v>
       </c>
@@ -4088,7 +4093,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>218</v>
       </c>
@@ -4098,7 +4103,7 @@
       <c r="C44" s="1"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>219</v>
       </c>
@@ -4108,7 +4113,7 @@
       <c r="C45" s="1"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <v>250</v>
       </c>
@@ -4125,22 +4130,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>288</v>
       </c>
@@ -4154,7 +4159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4166,7 +4171,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -4178,7 +4183,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -4190,7 +4195,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -4202,7 +4207,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -4214,7 +4219,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -4226,7 +4231,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -4238,7 +4243,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -4250,7 +4255,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>15</v>
       </c>
@@ -4262,7 +4267,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>16</v>
       </c>
@@ -4274,7 +4279,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>17</v>
       </c>
@@ -4286,7 +4291,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>18</v>
       </c>
@@ -4298,7 +4303,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>19</v>
       </c>
@@ -4310,7 +4315,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>20</v>
       </c>
@@ -4322,7 +4327,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>21</v>
       </c>
@@ -4334,7 +4339,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>190</v>
       </c>
@@ -4346,7 +4351,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>191</v>
       </c>
@@ -4358,7 +4363,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>192</v>
       </c>
@@ -4370,7 +4375,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>193</v>
       </c>
@@ -4382,7 +4387,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>194</v>
       </c>
@@ -4394,7 +4399,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>195</v>
       </c>
@@ -4406,7 +4411,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>196</v>
       </c>
@@ -4418,7 +4423,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>198</v>
       </c>
@@ -4430,7 +4435,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>200</v>
       </c>
@@ -4440,7 +4445,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>201</v>
       </c>
@@ -4450,7 +4455,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>202</v>
       </c>
@@ -4460,7 +4465,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>203</v>
       </c>
@@ -4470,7 +4475,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>205</v>
       </c>
@@ -4480,7 +4485,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>210</v>
       </c>
@@ -4490,7 +4495,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>211</v>
       </c>
@@ -4500,7 +4505,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>215</v>
       </c>
@@ -4510,7 +4515,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>216</v>
       </c>
@@ -4520,7 +4525,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>217</v>
       </c>
@@ -4530,7 +4535,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>218</v>
       </c>
@@ -4540,7 +4545,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>219</v>
       </c>
@@ -4550,7 +4555,7 @@
       <c r="C36" s="1"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>250</v>
       </c>
@@ -4567,22 +4572,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>288</v>
       </c>
@@ -4596,7 +4601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>113</v>
       </c>
@@ -4608,7 +4613,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>114</v>
       </c>
@@ -4620,7 +4625,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>115</v>
       </c>
@@ -4632,7 +4637,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>116</v>
       </c>
@@ -4644,7 +4649,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>117</v>
       </c>
@@ -4656,7 +4661,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>118</v>
       </c>
@@ -4668,7 +4673,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>119</v>
       </c>
@@ -4680,7 +4685,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>120</v>
       </c>
@@ -4692,7 +4697,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>121</v>
       </c>
@@ -4704,7 +4709,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>122</v>
       </c>
@@ -4716,7 +4721,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>123</v>
       </c>
@@ -4728,7 +4733,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>124</v>
       </c>
@@ -4740,7 +4745,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>125</v>
       </c>
@@ -4752,7 +4757,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>126</v>
       </c>
@@ -4764,7 +4769,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>129</v>
       </c>
@@ -4776,7 +4781,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>130</v>
       </c>
@@ -4788,7 +4793,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>131</v>
       </c>
@@ -4800,7 +4805,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>132</v>
       </c>
@@ -4812,7 +4817,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>138</v>
       </c>
@@ -4824,7 +4829,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>139</v>
       </c>
@@ -4836,7 +4841,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>140</v>
       </c>
@@ -4848,7 +4853,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>141</v>
       </c>
@@ -4860,7 +4865,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>142</v>
       </c>
@@ -4872,7 +4877,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>143</v>
       </c>
@@ -4884,7 +4889,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>144</v>
       </c>
@@ -4896,7 +4901,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>145</v>
       </c>
@@ -4908,7 +4913,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>146</v>
       </c>
@@ -4920,7 +4925,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>147</v>
       </c>
@@ -4932,7 +4937,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>148</v>
       </c>
@@ -4944,7 +4949,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>149</v>
       </c>
@@ -4956,7 +4961,7 @@
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>150</v>
       </c>
@@ -4968,7 +4973,7 @@
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>151</v>
       </c>
@@ -4980,7 +4985,7 @@
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>152</v>
       </c>
@@ -4992,7 +4997,7 @@
       </c>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>153</v>
       </c>
@@ -5004,7 +5009,7 @@
       </c>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>154</v>
       </c>
@@ -5016,7 +5021,7 @@
       </c>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>155</v>
       </c>
@@ -5028,7 +5033,7 @@
       </c>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>156</v>
       </c>
@@ -5040,7 +5045,7 @@
       </c>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>190</v>
       </c>
@@ -5052,7 +5057,7 @@
       </c>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>191</v>
       </c>
@@ -5064,7 +5069,7 @@
       </c>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>192</v>
       </c>
@@ -5076,7 +5081,7 @@
       </c>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>193</v>
       </c>
@@ -5088,7 +5093,7 @@
       </c>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>194</v>
       </c>
@@ -5100,7 +5105,7 @@
       </c>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>195</v>
       </c>
@@ -5112,7 +5117,7 @@
       </c>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>198</v>
       </c>
@@ -5124,7 +5129,7 @@
       </c>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>200</v>
       </c>
@@ -5134,7 +5139,7 @@
       <c r="C46" s="1"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>201</v>
       </c>
@@ -5144,7 +5149,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>202</v>
       </c>
@@ -5154,7 +5159,7 @@
       <c r="C48" s="1"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>203</v>
       </c>
@@ -5164,7 +5169,7 @@
       <c r="C49" s="1"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>205</v>
       </c>
@@ -5174,7 +5179,7 @@
       <c r="C50" s="1"/>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>210</v>
       </c>
@@ -5186,7 +5191,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>211</v>
       </c>
@@ -5196,7 +5201,7 @@
       <c r="C52" s="1"/>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>215</v>
       </c>
@@ -5206,7 +5211,7 @@
       <c r="C53" s="1"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>216</v>
       </c>
@@ -5216,7 +5221,7 @@
       <c r="C54" s="1"/>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>217</v>
       </c>
@@ -5226,7 +5231,7 @@
       <c r="C55" s="1"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>218</v>
       </c>
@@ -5236,7 +5241,7 @@
       <c r="C56" s="1"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>219</v>
       </c>
@@ -5246,7 +5251,7 @@
       <c r="C57" s="1"/>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>250</v>
       </c>
@@ -5256,7 +5261,7 @@
       <c r="C58" s="9"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>210</v>
       </c>
@@ -5271,22 +5276,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>288</v>
       </c>
@@ -5300,7 +5305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -5312,7 +5317,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -5324,7 +5329,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -5336,7 +5341,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -5348,7 +5353,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -5360,7 +5365,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -5372,7 +5377,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -5384,7 +5389,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -5396,7 +5401,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -5408,7 +5413,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -5420,7 +5425,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -5432,7 +5437,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -5444,7 +5449,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>89</v>
       </c>
@@ -5456,7 +5461,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>90</v>
       </c>
@@ -5468,7 +5473,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>91</v>
       </c>
@@ -5480,7 +5485,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>92</v>
       </c>
@@ -5492,7 +5497,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>93</v>
       </c>
@@ -5504,7 +5509,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>94</v>
       </c>
@@ -5516,7 +5521,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>95</v>
       </c>
@@ -5528,7 +5533,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>96</v>
       </c>
@@ -5540,7 +5545,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>97</v>
       </c>
@@ -5552,7 +5557,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>98</v>
       </c>
@@ -5564,7 +5569,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>99</v>
       </c>
@@ -5576,7 +5581,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>100</v>
       </c>
@@ -5588,7 +5593,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>101</v>
       </c>
@@ -5600,7 +5605,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>102</v>
       </c>
@@ -5612,7 +5617,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>103</v>
       </c>
@@ -5624,7 +5629,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>104</v>
       </c>
@@ -5636,7 +5641,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>105</v>
       </c>
@@ -5648,7 +5653,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>106</v>
       </c>
@@ -5660,7 +5665,7 @@
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>107</v>
       </c>
@@ -5672,7 +5677,7 @@
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>108</v>
       </c>
@@ -5684,7 +5689,7 @@
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>109</v>
       </c>
@@ -5696,7 +5701,7 @@
       </c>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>110</v>
       </c>
@@ -5708,7 +5713,7 @@
       </c>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>111</v>
       </c>
@@ -5720,7 +5725,7 @@
       </c>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>112</v>
       </c>
@@ -5732,7 +5737,7 @@
       </c>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>113</v>
       </c>
@@ -5744,7 +5749,7 @@
       </c>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>114</v>
       </c>
@@ -5756,7 +5761,7 @@
       </c>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>115</v>
       </c>
@@ -5768,7 +5773,7 @@
       </c>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>116</v>
       </c>
@@ -5780,7 +5785,7 @@
       </c>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>117</v>
       </c>
@@ -5792,7 +5797,7 @@
       </c>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>190</v>
       </c>
@@ -5804,7 +5809,7 @@
       </c>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>191</v>
       </c>
@@ -5816,7 +5821,7 @@
       </c>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>192</v>
       </c>
@@ -5828,7 +5833,7 @@
       </c>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>193</v>
       </c>
@@ -5840,7 +5845,7 @@
       </c>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>194</v>
       </c>
@@ -5852,7 +5857,7 @@
       </c>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>195</v>
       </c>
@@ -5864,7 +5869,7 @@
       </c>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>196</v>
       </c>
@@ -5876,7 +5881,7 @@
       </c>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>197</v>
       </c>
@@ -5888,7 +5893,7 @@
       </c>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>198</v>
       </c>
@@ -5900,7 +5905,7 @@
       </c>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>200</v>
       </c>
@@ -5910,7 +5915,7 @@
       <c r="C52" s="1"/>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>201</v>
       </c>
@@ -5920,7 +5925,7 @@
       <c r="C53" s="1"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>202</v>
       </c>
@@ -5930,7 +5935,7 @@
       <c r="C54" s="1"/>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>203</v>
       </c>
@@ -5940,7 +5945,7 @@
       <c r="C55" s="1"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>205</v>
       </c>
@@ -5950,7 +5955,7 @@
       <c r="C56" s="1"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>210</v>
       </c>
@@ -5962,7 +5967,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>211</v>
       </c>
@@ -5972,7 +5977,7 @@
       <c r="C58" s="1"/>
       <c r="D58" s="6"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>215</v>
       </c>
@@ -5982,7 +5987,7 @@
       <c r="C59" s="1"/>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>216</v>
       </c>
@@ -5992,7 +5997,7 @@
       <c r="C60" s="1"/>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>217</v>
       </c>
@@ -6002,7 +6007,7 @@
       <c r="C61" s="1"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>218</v>
       </c>
@@ -6012,7 +6017,7 @@
       <c r="C62" s="1"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>219</v>
       </c>
@@ -6022,7 +6027,7 @@
       <c r="C63" s="1"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>250</v>
       </c>
@@ -6039,21 +6044,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="3" max="4" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="26.875" customWidth="1"/>
+    <col min="3" max="4" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>288</v>
       </c>
@@ -6067,7 +6072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>113</v>
       </c>
@@ -6079,7 +6084,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>114</v>
       </c>
@@ -6091,7 +6096,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>115</v>
       </c>
@@ -6103,7 +6108,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>116</v>
       </c>
@@ -6115,7 +6120,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>118</v>
       </c>
@@ -6127,7 +6132,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>119</v>
       </c>
@@ -6139,7 +6144,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>120</v>
       </c>
@@ -6151,7 +6156,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>121</v>
       </c>
@@ -6163,7 +6168,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>122</v>
       </c>
@@ -6175,7 +6180,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>123</v>
       </c>
@@ -6187,7 +6192,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>124</v>
       </c>
@@ -6199,7 +6204,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>125</v>
       </c>
@@ -6211,7 +6216,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>126</v>
       </c>
@@ -6223,7 +6228,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>127</v>
       </c>
@@ -6235,7 +6240,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>128</v>
       </c>
@@ -6247,7 +6252,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>129</v>
       </c>
@@ -6259,7 +6264,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>130</v>
       </c>
@@ -6271,7 +6276,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>131</v>
       </c>
@@ -6283,7 +6288,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>132</v>
       </c>
@@ -6295,7 +6300,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>133</v>
       </c>
@@ -6307,7 +6312,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>134</v>
       </c>
@@ -6319,7 +6324,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>135</v>
       </c>
@@ -6331,7 +6336,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>136</v>
       </c>
@@ -6343,7 +6348,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>137</v>
       </c>
@@ -6355,7 +6360,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>140</v>
       </c>
@@ -6367,7 +6372,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>141</v>
       </c>
@@ -6379,7 +6384,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>142</v>
       </c>
@@ -6391,7 +6396,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>143</v>
       </c>
@@ -6403,7 +6408,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>190</v>
       </c>
@@ -6415,7 +6420,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>191</v>
       </c>
@@ -6427,7 +6432,7 @@
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>192</v>
       </c>
@@ -6439,7 +6444,7 @@
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>193</v>
       </c>
@@ -6451,7 +6456,7 @@
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>194</v>
       </c>
@@ -6463,7 +6468,7 @@
       </c>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>195</v>
       </c>
@@ -6475,7 +6480,7 @@
       </c>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>198</v>
       </c>
@@ -6487,7 +6492,7 @@
       </c>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>200</v>
       </c>
@@ -6497,7 +6502,7 @@
       <c r="C37" s="1"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>201</v>
       </c>
@@ -6507,7 +6512,7 @@
       <c r="C38" s="1"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>202</v>
       </c>
@@ -6517,7 +6522,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>203</v>
       </c>
@@ -6527,7 +6532,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>205</v>
       </c>
@@ -6537,7 +6542,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>210</v>
       </c>
@@ -6547,7 +6552,7 @@
       <c r="C42" s="1"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>211</v>
       </c>
@@ -6557,7 +6562,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>215</v>
       </c>
@@ -6567,7 +6572,7 @@
       <c r="C44" s="1"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>216</v>
       </c>
@@ -6577,7 +6582,7 @@
       <c r="C45" s="1"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>217</v>
       </c>
@@ -6587,7 +6592,7 @@
       <c r="C46" s="1"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>218</v>
       </c>
@@ -6597,7 +6602,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>219</v>
       </c>
@@ -6607,7 +6612,7 @@
       <c r="C48" s="1"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>250</v>
       </c>

</xml_diff>